<commit_message>
Updated Plugin And Framework Code (Ali Abbas)
</commit_message>
<xml_diff>
--- a/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/IBBillPayment.xlsx
+++ b/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/IBBillPayment.xlsx
@@ -30,9 +30,6 @@
     <t>status_query</t>
   </si>
   <si>
-    <t>DB_Value</t>
-  </si>
-  <si>
     <t>OTP_Value</t>
   </si>
   <si>
@@ -60,12 +57,6 @@
     <t>SELECT DT.TRANSACTION_AMOUNT FROM DC_TRANSACTION DT WHERE DT.TRANSACTION_ID = '</t>
   </si>
   <si>
-    <t>QAT_BPS</t>
-  </si>
-  <si>
-    <t>QADB</t>
-  </si>
-  <si>
     <t>SELECT DT.BILL_COMPANY FROM DC_TRANSACTION DT WHERE DT.TRANSACTION_ID = '</t>
   </si>
   <si>
@@ -100,6 +91,15 @@
   </si>
   <si>
     <t>pakistan3</t>
+  </si>
+  <si>
+    <t>DIGITAL_CHANNEL_SEC</t>
+  </si>
+  <si>
+    <t>status_query2</t>
+  </si>
+  <si>
+    <t>BEGIN UPDATE DC_SCHEDULED_TRAN_MASTER STM SET STM.STATE = 46 , STM.IS_DELETED = 1 WHERE STM.BILL_BENEFICIARY_ID = (SELECT BPB.BENEFICIARY_ID FROM DC_BILL_PAYMENT_BENEFICIARY BPB WHERE BPB.CONSUMER_NUMBER = '0400000069505' AND BPB.CUSTOMER_INFO_ID = (SELECT CI.CUSTOMER_INFO_ID FROM DC_CUSTOMER_INFO CI WHERE CI.CUSTOMER_NAME = 'ABBY') AND BPB.IS_ACTIVE = 1);COMMIT;END;</t>
   </si>
 </sst>
 </file>
@@ -427,13 +427,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="44.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44.42578125" style="1" customWidth="1"/>
@@ -453,40 +455,40 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
       <c r="N1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -494,43 +496,43 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="H2">
         <v>12345</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" t="s">
-        <v>15</v>
-      </c>
       <c r="M2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="N2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BillPayment Color Issue
</commit_message>
<xml_diff>
--- a/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/IBBillPayment.xlsx
+++ b/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/IBBillPayment.xlsx
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Inquiry Next Button Fix
</commit_message>
<xml_diff>
--- a/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/IBBillPayment.xlsx
+++ b/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/IBBillPayment.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="60">
   <si>
     <t>Case</t>
   </si>
@@ -135,9 +135,6 @@
     <t>When valid bill details are provided 05151110478500</t>
   </si>
   <si>
-    <t>BEGIN UPDATE DC_SCHEDULED_TRAN_MASTER STM SET STM.STATE = 46 , STM.IS_DELETED = 1 WHERE STM.BILL_BENEFICIARY_ID = (SELECT BPB.BENEFICIARY_ID FROM DC_BILL_PAYMENT_BENEFICIARY BPB WHERE BPB.CONSUMER_NUMBER = '{ConsumerNo}' AND BPB.CUSTOMER_INFO_ID = (SELECT CI.CUSTOMER_INFO_ID FROM DC_CUSTOMER_INFO CI WHERE CI.CUSTOMER_NAME = 'ABBY') AND BPB.IS_ACTIVE = 1);UPDATE DC_BILL_PAYMENT_BENEFICIARY DPB SET DPB.IS_SI_SCHEDULED = 0,DPB.IS_ACTIVE = 0 WHERE DPB.CONSUMER_NUMBER = '{ConsumerNo}' AND DPB.CUSTOMER_INFO_ID = (SELECT CI.CUSTOMER_INFO_ID FROM DC_CUSTOMER_INFO CI WHERE CI.CUSTOMER_NAME = 'A7575254900') AND DPB.IS_ACTIVE = 1;COMMIT;END;</t>
-  </si>
-  <si>
     <t>05151110478500</t>
   </si>
   <si>
@@ -172,6 +169,36 @@
   </si>
   <si>
     <t>Abby</t>
+  </si>
+  <si>
+    <t>schedule_config</t>
+  </si>
+  <si>
+    <t>Select PARAMTER_VALUE from DC_APPLICATION_PARAM_DETAIL i where I.APPLICATION_PARAMETER_ID='906'</t>
+  </si>
+  <si>
+    <t>schedule_verify</t>
+  </si>
+  <si>
+    <t>Select FIRST_EXECUTION_DATE, LAST_EXECUTION_DATE from DC_SCHEDULED_TRAN_MASTER i where I.CUSTOMER_INFO_ID='{customer_info_id}'</t>
+  </si>
+  <si>
+    <t>01266110067304</t>
+  </si>
+  <si>
+    <t>BEGIN UPDATE DC_SCHEDULED_TRAN_MASTER STM SET STM.STATE = 46 , STM.IS_DELETED = 1 WHERE STM.BILL_BENEFICIARY_ID = (SELECT BPB.BENEFICIARY_ID FROM DC_BILL_PAYMENT_BENEFICIARY BPB WHERE BPB.CONSUMER_NUMBER = '{ConsumerNo}' AND BPB.CUSTOMER_INFO_ID = (SELECT CI.CUSTOMER_INFO_ID FROM DC_CUSTOMER_INFO CI WHERE CI.CUSTOMER_NAME = 'ABBY') AND BPB.IS_ACTIVE = 1);UPDATE DC_BILL_PAYMENT_BENEFICIARY DPB SET DPB.IS_SI_SCHEDULED = 0,DPB.IS_ACTIVE = 0 WHERE DPB.CONSUMER_NUMBER = '{ConsumerNo}' AND DPB.CUSTOMER_INFO_ID = (SELECT CI.CUSTOMER_INFO_ID FROM DC_CUSTOMER_INFO CI WHERE CI.CUSTOMER_NAME = 'ABBY') AND DPB.IS_ACTIVE = 1;COMMIT;END;</t>
+  </si>
+  <si>
+    <t>When valid bill details are provided 01266110067304</t>
+  </si>
+  <si>
+    <t>02197900643103</t>
+  </si>
+  <si>
+    <t>PESCO</t>
+  </si>
+  <si>
+    <t>PESCO001</t>
   </si>
 </sst>
 </file>
@@ -501,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +540,7 @@
     <col min="7" max="7" width="127.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="185.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16.140625" style="4" customWidth="1"/>
     <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="39.42578125" bestFit="1" customWidth="1"/>
@@ -521,9 +548,11 @@
     <col min="23" max="23" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="139.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="118.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="101.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="132.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -579,7 +608,7 @@
         <v>27</v>
       </c>
       <c r="S1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T1" t="s">
         <v>34</v>
@@ -597,10 +626,16 @@
         <v>33</v>
       </c>
       <c r="Y1" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -608,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>30</v>
@@ -617,7 +652,7 @@
         <v>35</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>26</v>
@@ -652,34 +687,40 @@
       <c r="Q2" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="4">
-        <v>25417000018103</v>
+      <c r="R2" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U2" t="s">
         <v>31</v>
       </c>
       <c r="W2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y2" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>30</v>
@@ -688,7 +729,7 @@
         <v>35</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>26</v>
@@ -723,37 +764,43 @@
       <c r="Q3" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="4">
-        <v>25417000018103</v>
+      <c r="R3" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V3">
         <v>1000</v>
       </c>
       <c r="W3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y3" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>30</v>
@@ -762,7 +809,7 @@
         <v>35</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>26</v>
@@ -797,24 +844,110 @@
       <c r="Q4" t="s">
         <v>21</v>
       </c>
-      <c r="R4" s="4">
-        <v>25417523618103</v>
+      <c r="R4" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U4" t="s">
         <v>31</v>
       </c>
       <c r="W4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5">
+        <v>12345678</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="U5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W5" t="s">
         <v>49</v>
       </c>
+      <c r="X5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="R7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Commit for Kumail Solution
</commit_message>
<xml_diff>
--- a/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/IBBillPayment.xlsx
+++ b/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/IBBillPayment.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="83">
   <si>
     <t>Case</t>
   </si>
@@ -222,12 +222,6 @@
     <t>NQESCO01</t>
   </si>
   <si>
-    <t>04030023521301</t>
-  </si>
-  <si>
-    <t>04037900493703</t>
-  </si>
-  <si>
     <t>Home</t>
   </si>
   <si>
@@ -265,6 +259,15 @@
   </si>
   <si>
     <t>is_partial_payment_query</t>
+  </si>
+  <si>
+    <t>28156121235512</t>
+  </si>
+  <si>
+    <t>When valid bill details are provided 28156121235512</t>
+  </si>
+  <si>
+    <t>00476000949001 | SHAISTA | HBL ANNEXE.</t>
   </si>
 </sst>
 </file>
@@ -594,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF6"/>
+  <dimension ref="A1:AF7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AF9" sqref="AF9"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +612,7 @@
     <col min="7" max="7" width="140.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="185.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="38.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16.140625" style="4" customWidth="1"/>
     <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="39.42578125" bestFit="1" customWidth="1"/>
@@ -709,19 +712,19 @@
         <v>47</v>
       </c>
       <c r="AB1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AC1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD1" t="s">
         <v>75</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>77</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>79</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -744,7 +747,7 @@
         <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>35</v>
@@ -777,7 +780,7 @@
         <v>21</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>42</v>
@@ -801,19 +804,19 @@
         <v>49</v>
       </c>
       <c r="AB2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AC2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD2" t="s">
         <v>74</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>76</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>78</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
@@ -836,7 +839,7 @@
         <v>50</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>63</v>
@@ -869,13 +872,13 @@
         <v>21</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>42</v>
       </c>
       <c r="W3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="X3" t="s">
         <v>41</v>
@@ -890,19 +893,19 @@
         <v>49</v>
       </c>
       <c r="AB3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AC3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD3" t="s">
         <v>74</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>76</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>78</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
@@ -925,7 +928,7 @@
         <v>51</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>64</v>
@@ -958,7 +961,7 @@
         <v>21</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>42</v>
@@ -967,7 +970,7 @@
         <v>30</v>
       </c>
       <c r="W4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="X4" t="s">
         <v>41</v>
@@ -982,19 +985,19 @@
         <v>49</v>
       </c>
       <c r="AB4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AC4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD4" t="s">
         <v>74</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>76</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>78</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -1017,7 +1020,7 @@
         <v>52</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>65</v>
@@ -1050,7 +1053,7 @@
         <v>21</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="S5" s="4" t="s">
         <v>42</v>
@@ -1074,19 +1077,19 @@
         <v>49</v>
       </c>
       <c r="AB5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AC5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD5" t="s">
         <v>74</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>76</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>78</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
@@ -1109,7 +1112,7 @@
         <v>53</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>66</v>
@@ -1142,7 +1145,7 @@
         <v>21</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="S6" s="4" t="s">
         <v>42</v>
@@ -1163,19 +1166,108 @@
         <v>49</v>
       </c>
       <c r="AB6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AC6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD6" t="s">
         <v>74</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>76</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>78</v>
       </c>
-      <c r="AF6" t="s">
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>80</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7">
+        <v>12345682</v>
+      </c>
+      <c r="J7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P7" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="U7" t="s">
+        <v>30</v>
+      </c>
+      <c r="X7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>